<commit_message>
Create db insert & install mysql + express
</commit_message>
<xml_diff>
--- a/database/MENU.xlsx
+++ b/database/MENU.xlsx
@@ -411,10 +411,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>메뉴번호(VARCHAR2(200))</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>메뉴카테고리(VARCHAR2(500))</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -868,6 +864,10 @@
   </si>
   <si>
     <t>오곡 버블티</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메뉴번호(int)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -875,7 +875,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1267,11 +1267,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="25.125" customWidth="1"/>
     <col min="2" max="2" width="28.875" customWidth="1"/>
@@ -1285,18 +1285,18 @@
     <col min="10" max="10" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="8" t="s">
         <v>122</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>123</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -1304,13 +1304,13 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="D2" s="3">
         <v>3000</v>
@@ -1321,13 +1321,13 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>127</v>
       </c>
       <c r="D3" s="3">
         <v>2500</v>
@@ -1338,13 +1338,13 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D4" s="3">
         <v>3500</v>
@@ -1355,13 +1355,13 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D5" s="3">
         <v>3000</v>
@@ -1372,13 +1372,13 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D6" s="3">
         <v>3500</v>
@@ -1389,13 +1389,13 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D7" s="3">
         <v>3000</v>
@@ -1406,13 +1406,13 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D8" s="3">
         <v>4000</v>
@@ -1423,13 +1423,13 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D9" s="3">
         <v>3500</v>
@@ -1440,13 +1440,13 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D10" s="3">
         <v>4000</v>
@@ -1457,13 +1457,13 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D11" s="3">
         <v>3500</v>
@@ -1474,13 +1474,13 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D12" s="3">
         <v>4000</v>
@@ -1491,13 +1491,13 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D13" s="3">
         <v>3500</v>
@@ -1508,13 +1508,13 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D14" s="3">
         <v>4800</v>
@@ -1525,13 +1525,13 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D15" s="3">
         <v>4800</v>
@@ -1542,13 +1542,13 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D16" s="3">
         <v>4500</v>
@@ -1559,13 +1559,13 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D17" s="3">
         <v>4500</v>
@@ -1576,13 +1576,13 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D18" s="3">
         <v>4000</v>
@@ -1593,13 +1593,13 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D19" s="3">
         <v>3500</v>
@@ -1610,13 +1610,13 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D20" s="3">
         <v>4500</v>
@@ -1627,13 +1627,13 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D21" s="3">
         <v>4500</v>
@@ -1644,13 +1644,13 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>147</v>
       </c>
       <c r="D22" s="3">
         <v>9800</v>
@@ -1661,13 +1661,13 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D23" s="3">
         <v>10800</v>
@@ -1678,13 +1678,13 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D24" s="3">
         <v>11800</v>
@@ -1695,13 +1695,13 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D25" s="3">
         <v>11800</v>
@@ -1712,13 +1712,13 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D26" s="3">
         <v>12800</v>
@@ -1729,13 +1729,13 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>153</v>
       </c>
       <c r="D27" s="3">
         <v>4000</v>
@@ -1746,13 +1746,13 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D28" s="3">
         <v>4500</v>
@@ -1763,13 +1763,13 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D29" s="3">
         <v>4500</v>
@@ -1780,13 +1780,13 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9">
       <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D30" s="3">
         <v>4900</v>
@@ -1797,13 +1797,13 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D31" s="3">
         <v>4000</v>
@@ -1814,13 +1814,13 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D32" s="3">
         <v>4900</v>
@@ -1831,13 +1831,13 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D33" s="3">
         <v>5500</v>
@@ -1848,13 +1848,13 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D34" s="3">
         <v>4500</v>
@@ -1865,13 +1865,13 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D35" s="3">
         <v>4500</v>
@@ -1882,13 +1882,13 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9">
       <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D36" s="3">
         <v>4500</v>
@@ -1899,13 +1899,13 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D37" s="3">
         <v>4500</v>
@@ -1916,13 +1916,13 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D38" s="3">
         <v>4500</v>
@@ -1933,13 +1933,13 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D39" s="3">
         <v>4100</v>
@@ -1950,13 +1950,13 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9">
       <c r="A40" s="1"/>
       <c r="B40" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D40" s="3">
         <v>4100</v>
@@ -1967,13 +1967,13 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9">
       <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D41" s="3">
         <v>4100</v>
@@ -1984,13 +1984,13 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D42" s="3">
         <v>4500</v>
@@ -2001,13 +2001,13 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9">
       <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D43" s="3">
         <v>4500</v>
@@ -2018,13 +2018,13 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9">
       <c r="A44" s="1"/>
       <c r="B44" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D44" s="3">
         <v>4500</v>
@@ -2035,13 +2035,13 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9">
       <c r="A45" s="1"/>
       <c r="B45" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D45" s="3">
         <v>4500</v>
@@ -2052,13 +2052,13 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9">
       <c r="A46" s="1"/>
       <c r="B46" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>169</v>
       </c>
       <c r="D46" s="3">
         <v>4500</v>
@@ -2069,13 +2069,13 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9">
       <c r="A47" s="1"/>
       <c r="B47" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D47" s="3">
         <v>5500</v>
@@ -2086,13 +2086,13 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9">
       <c r="A48" s="1"/>
       <c r="B48" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D48" s="3">
         <v>4500</v>
@@ -2103,13 +2103,13 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9">
       <c r="A49" s="1"/>
       <c r="B49" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D49" s="3">
         <v>4500</v>
@@ -2120,13 +2120,13 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9">
       <c r="A50" s="1"/>
       <c r="B50" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D50" s="3">
         <v>4500</v>
@@ -2137,13 +2137,13 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9">
       <c r="A51" s="1"/>
       <c r="B51" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>179</v>
       </c>
       <c r="D51" s="3">
         <v>5900</v>
@@ -2154,13 +2154,13 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9">
       <c r="A52" s="1"/>
       <c r="B52" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D52" s="3">
         <v>5900</v>
@@ -2171,13 +2171,13 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9">
       <c r="A53" s="1"/>
       <c r="B53" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D53" s="3">
         <v>4800</v>
@@ -2188,13 +2188,13 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9">
       <c r="A54" s="1"/>
       <c r="B54" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D54" s="3">
         <v>4800</v>
@@ -2205,13 +2205,13 @@
       <c r="H54" s="1"/>
       <c r="I54" s="2"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9">
       <c r="A55" s="1"/>
       <c r="B55" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D55" s="3">
         <v>4800</v>
@@ -2222,13 +2222,13 @@
       <c r="H55" s="1"/>
       <c r="I55" s="4"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9">
       <c r="A56" s="1"/>
       <c r="B56" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D56" s="3">
         <v>4800</v>
@@ -2239,13 +2239,13 @@
       <c r="H56" s="1"/>
       <c r="I56" s="4"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9">
       <c r="A57" s="1"/>
       <c r="B57" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D57" s="3">
         <v>4800</v>
@@ -2256,13 +2256,13 @@
       <c r="H57" s="1"/>
       <c r="I57" s="4"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9">
       <c r="A58" s="1"/>
       <c r="B58" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D58" s="3">
         <v>4800</v>
@@ -2273,13 +2273,13 @@
       <c r="H58" s="1"/>
       <c r="I58" s="4"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9">
       <c r="A59" s="1"/>
       <c r="B59" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D59" s="3">
         <v>4800</v>
@@ -2290,13 +2290,13 @@
       <c r="H59" s="1"/>
       <c r="I59" s="4"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9">
       <c r="A60" s="1"/>
       <c r="B60" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D60" s="3">
         <v>4800</v>
@@ -2307,13 +2307,13 @@
       <c r="H60" s="1"/>
       <c r="I60" s="4"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9">
       <c r="A61" s="1"/>
       <c r="B61" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D61" s="3">
         <v>4300</v>
@@ -2324,13 +2324,13 @@
       <c r="H61" s="1"/>
       <c r="I61" s="4"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9">
       <c r="A62" s="1"/>
       <c r="B62" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D62" s="3">
         <v>4300</v>
@@ -2341,13 +2341,13 @@
       <c r="H62" s="1"/>
       <c r="I62" s="4"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9">
       <c r="A63" s="1"/>
       <c r="B63" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D63" s="3">
         <v>4800</v>
@@ -2358,13 +2358,13 @@
       <c r="H63" s="1"/>
       <c r="I63" s="4"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9">
       <c r="A64" s="1"/>
       <c r="B64" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D64" s="3">
         <v>4800</v>
@@ -2375,13 +2375,13 @@
       <c r="H64" s="1"/>
       <c r="I64" s="4"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9">
       <c r="A65" s="1"/>
       <c r="B65" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D65" s="3">
         <v>3000</v>
@@ -2392,13 +2392,13 @@
       <c r="H65" s="1"/>
       <c r="I65" s="4"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9">
       <c r="A66" s="1"/>
       <c r="B66" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D66" s="3">
         <v>3000</v>
@@ -2409,13 +2409,13 @@
       <c r="H66" s="1"/>
       <c r="I66" s="4"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9">
       <c r="A67" s="1"/>
       <c r="B67" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C67" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>196</v>
       </c>
       <c r="D67" s="3">
         <v>6500</v>
@@ -2426,13 +2426,13 @@
       <c r="H67" s="1"/>
       <c r="I67" s="4"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9">
       <c r="A68" s="1"/>
       <c r="B68" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D68" s="3">
         <v>5900</v>
@@ -2443,13 +2443,13 @@
       <c r="H68" s="1"/>
       <c r="I68" s="4"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9">
       <c r="A69" s="1"/>
       <c r="B69" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D69" s="3">
         <v>5900</v>
@@ -2460,13 +2460,13 @@
       <c r="H69" s="1"/>
       <c r="I69" s="4"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9">
       <c r="A70" s="1"/>
       <c r="B70" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D70" s="3">
         <v>4500</v>
@@ -2477,13 +2477,13 @@
       <c r="H70" s="1"/>
       <c r="I70" s="4"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9">
       <c r="A71" s="1"/>
       <c r="B71" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D71" s="3">
         <v>4500</v>
@@ -2494,13 +2494,13 @@
       <c r="H71" s="1"/>
       <c r="I71" s="4"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9">
       <c r="A72" s="1"/>
       <c r="B72" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D72" s="3">
         <v>5900</v>
@@ -2511,13 +2511,13 @@
       <c r="H72" s="1"/>
       <c r="I72" s="4"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9">
       <c r="A73" s="1"/>
       <c r="B73" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D73" s="3">
         <v>3900</v>
@@ -2528,13 +2528,13 @@
       <c r="H73" s="1"/>
       <c r="I73" s="4"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9">
       <c r="A74" s="1"/>
       <c r="B74" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D74" s="3">
         <v>3900</v>
@@ -2545,13 +2545,13 @@
       <c r="H74" s="1"/>
       <c r="I74" s="4"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9">
       <c r="A75" s="1"/>
       <c r="B75" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D75" s="3">
         <v>4800</v>
@@ -2562,13 +2562,13 @@
       <c r="H75" s="1"/>
       <c r="I75" s="4"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9">
       <c r="A76" s="1"/>
       <c r="B76" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D76" s="3">
         <v>4300</v>
@@ -2579,13 +2579,13 @@
       <c r="H76" s="1"/>
       <c r="I76" s="4"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9">
       <c r="A77" s="1"/>
       <c r="B77" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D77" s="3">
         <v>1200</v>
@@ -2596,13 +2596,13 @@
       <c r="H77" s="1"/>
       <c r="I77" s="4"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9">
       <c r="A78" s="1"/>
       <c r="B78" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D78" s="3">
         <v>1200</v>
@@ -2613,13 +2613,13 @@
       <c r="H78" s="1"/>
       <c r="I78" s="4"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9">
       <c r="A79" s="1"/>
       <c r="B79" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D79" s="3">
         <v>3500</v>
@@ -2630,13 +2630,13 @@
       <c r="H79" s="1"/>
       <c r="I79" s="4"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9">
       <c r="A80" s="1"/>
       <c r="B80" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D80" s="3">
         <v>4500</v>
@@ -2647,13 +2647,13 @@
       <c r="H80" s="1"/>
       <c r="I80" s="4"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9">
       <c r="A81" s="1"/>
       <c r="B81" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D81" s="3">
         <v>3900</v>
@@ -2664,13 +2664,13 @@
       <c r="H81" s="1"/>
       <c r="I81" s="4"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9">
       <c r="A82" s="1"/>
       <c r="B82" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D82" s="3">
         <v>4500</v>
@@ -2681,13 +2681,13 @@
       <c r="H82" s="1"/>
       <c r="I82" s="4"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9">
       <c r="A83" s="1"/>
       <c r="B83" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D83" s="3">
         <v>3900</v>
@@ -2698,13 +2698,13 @@
       <c r="H83" s="1"/>
       <c r="I83" s="2"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9">
       <c r="A84" s="1"/>
       <c r="B84" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C84" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>214</v>
       </c>
       <c r="D84" s="3">
         <v>2500</v>
@@ -2715,13 +2715,13 @@
       <c r="H84" s="1"/>
       <c r="I84" s="2"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9">
       <c r="A85" s="1"/>
       <c r="B85" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D85" s="3">
         <v>2500</v>
@@ -2732,13 +2732,13 @@
       <c r="H85" s="1"/>
       <c r="I85" s="2"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9">
       <c r="A86" s="1"/>
       <c r="B86" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D86" s="3">
         <v>2500</v>
@@ -2749,13 +2749,13 @@
       <c r="H86" s="1"/>
       <c r="I86" s="2"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9">
       <c r="A87" s="1"/>
       <c r="B87" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D87" s="3">
         <v>2500</v>
@@ -2766,13 +2766,13 @@
       <c r="H87" s="1"/>
       <c r="I87" s="2"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9">
       <c r="A88" s="1"/>
       <c r="B88" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D88" s="3">
         <v>10000</v>
@@ -2783,13 +2783,13 @@
       <c r="H88" s="1"/>
       <c r="I88" s="2"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9">
       <c r="A89" s="1"/>
       <c r="B89" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D89" s="3">
         <v>1500</v>
@@ -2800,13 +2800,13 @@
       <c r="H89" s="1"/>
       <c r="I89" s="2"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9">
       <c r="A90" s="1"/>
       <c r="B90" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D90" s="3">
         <v>1500</v>
@@ -2817,13 +2817,13 @@
       <c r="H90" s="1"/>
       <c r="I90" s="4"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9">
       <c r="A91" s="1"/>
       <c r="B91" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D91" s="3">
         <v>1500</v>
@@ -2834,13 +2834,13 @@
       <c r="H91" s="1"/>
       <c r="I91" s="4"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9">
       <c r="A92" s="1"/>
       <c r="B92" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D92" s="3">
         <v>1500</v>
@@ -2851,13 +2851,13 @@
       <c r="H92" s="1"/>
       <c r="I92" s="4"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9">
       <c r="A93" s="1"/>
       <c r="B93" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D93" s="3">
         <v>1500</v>
@@ -2868,13 +2868,13 @@
       <c r="H93" s="1"/>
       <c r="I93" s="4"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9">
       <c r="A94" s="1"/>
       <c r="B94" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D94" s="3">
         <v>1500</v>
@@ -2885,13 +2885,13 @@
       <c r="H94" s="1"/>
       <c r="I94" s="4"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9">
       <c r="A95" s="1"/>
       <c r="B95" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D95" s="3">
         <v>1500</v>
@@ -2902,13 +2902,13 @@
       <c r="H95" s="1"/>
       <c r="I95" s="4"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9">
       <c r="A96" s="1"/>
       <c r="B96" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D96" s="3">
         <v>1500</v>
@@ -2919,13 +2919,13 @@
       <c r="H96" s="1"/>
       <c r="I96" s="4"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9">
       <c r="A97" s="1"/>
       <c r="B97" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D97" s="3">
         <v>12000</v>
@@ -2936,13 +2936,13 @@
       <c r="H97" s="1"/>
       <c r="I97" s="2"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9">
       <c r="A98" s="1"/>
       <c r="B98" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C98" s="2" t="s">
         <v>228</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>229</v>
       </c>
       <c r="D98" s="3">
         <v>4500</v>
@@ -2953,13 +2953,13 @@
       <c r="H98" s="1"/>
       <c r="I98" s="2"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9">
       <c r="A99" s="1"/>
       <c r="B99" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D99" s="3">
         <v>4500</v>
@@ -2969,13 +2969,13 @@
       <c r="G99" s="1"/>
       <c r="H99" s="1"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9">
       <c r="A100" s="1"/>
       <c r="B100" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D100" s="3">
         <v>4500</v>
@@ -2986,13 +2986,13 @@
       <c r="H100" s="1"/>
       <c r="I100" s="1"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9">
       <c r="A101" s="1"/>
       <c r="B101" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D101" s="3">
         <v>4500</v>
@@ -3003,23 +3003,23 @@
       <c r="H101" s="1"/>
       <c r="I101" s="2"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9">
       <c r="B102" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D102" s="3">
         <v>4500</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9">
       <c r="B103" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D103" s="3">
         <v>4500</v>
@@ -3040,7 +3040,7 @@
       <selection activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="14.375" customWidth="1"/>
     <col min="2" max="2" width="10.375" customWidth="1"/>
@@ -3054,7 +3054,7 @@
     <col min="10" max="10" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3086,7 +3086,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -3105,7 +3105,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
@@ -3124,7 +3124,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="2" t="s">
@@ -3143,7 +3143,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
@@ -3162,7 +3162,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="2" t="s">
@@ -3181,7 +3181,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
@@ -3200,7 +3200,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
@@ -3219,7 +3219,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="2" t="s">
@@ -3238,7 +3238,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
@@ -3257,7 +3257,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
@@ -3276,7 +3276,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
@@ -3295,7 +3295,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="s">
@@ -3314,7 +3314,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
@@ -3333,7 +3333,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
@@ -3352,7 +3352,7 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
@@ -3371,7 +3371,7 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
@@ -3390,7 +3390,7 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="2" t="s">
@@ -3409,7 +3409,7 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
@@ -3428,7 +3428,7 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="2" t="s">
@@ -3447,7 +3447,7 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="2" t="s">
@@ -3466,7 +3466,7 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="2" t="s">
@@ -3485,7 +3485,7 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="2" t="s">
@@ -3504,7 +3504,7 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="2" t="s">
@@ -3523,7 +3523,7 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="2" t="s">
@@ -3542,7 +3542,7 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="2" t="s">
@@ -3561,7 +3561,7 @@
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="2" t="s">
@@ -3580,7 +3580,7 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="2" t="s">
@@ -3599,7 +3599,7 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:10" ht="33" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" ht="33">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="2" t="s">
@@ -3618,7 +3618,7 @@
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="2" t="s">
@@ -3637,7 +3637,7 @@
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="2" t="s">
@@ -3656,7 +3656,7 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="2" t="s">
@@ -3675,7 +3675,7 @@
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="2" t="s">
@@ -3694,7 +3694,7 @@
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="2" t="s">
@@ -3713,7 +3713,7 @@
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="2" t="s">
@@ -3732,7 +3732,7 @@
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="2" t="s">
@@ -3751,7 +3751,7 @@
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="2" t="s">
@@ -3770,7 +3770,7 @@
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="2" t="s">
@@ -3789,7 +3789,7 @@
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="2" t="s">
@@ -3808,7 +3808,7 @@
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="2" t="s">
@@ -3827,7 +3827,7 @@
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="2" t="s">
@@ -3846,7 +3846,7 @@
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="2" t="s">
@@ -3865,7 +3865,7 @@
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="2" t="s">
@@ -3884,7 +3884,7 @@
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="2" t="s">
@@ -3903,7 +3903,7 @@
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="2" t="s">
@@ -3922,7 +3922,7 @@
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="2" t="s">
@@ -3941,7 +3941,7 @@
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="2" t="s">
@@ -3960,7 +3960,7 @@
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="2" t="s">
@@ -3979,7 +3979,7 @@
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="2" t="s">
@@ -3998,7 +3998,7 @@
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="2" t="s">
@@ -4017,7 +4017,7 @@
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="2" t="s">
@@ -4036,7 +4036,7 @@
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="2" t="s">
@@ -4055,7 +4055,7 @@
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="2" t="s">
@@ -4074,7 +4074,7 @@
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="2" t="s">
@@ -4095,7 +4095,7 @@
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="2" t="s">
@@ -4114,7 +4114,7 @@
       <c r="I55" s="1"/>
       <c r="J55" s="4"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="2" t="s">
@@ -4133,7 +4133,7 @@
       <c r="I56" s="1"/>
       <c r="J56" s="4"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="2" t="s">
@@ -4152,7 +4152,7 @@
       <c r="I57" s="1"/>
       <c r="J57" s="4"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="2" t="s">
@@ -4171,7 +4171,7 @@
       <c r="I58" s="1"/>
       <c r="J58" s="4"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="2" t="s">
@@ -4190,7 +4190,7 @@
       <c r="I59" s="1"/>
       <c r="J59" s="4"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="2" t="s">
@@ -4209,7 +4209,7 @@
       <c r="I60" s="1"/>
       <c r="J60" s="4"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="2" t="s">
@@ -4228,7 +4228,7 @@
       <c r="I61" s="1"/>
       <c r="J61" s="4"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="2" t="s">
@@ -4247,7 +4247,7 @@
       <c r="I62" s="1"/>
       <c r="J62" s="4"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="2" t="s">
@@ -4266,7 +4266,7 @@
       <c r="I63" s="1"/>
       <c r="J63" s="4"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="2" t="s">
@@ -4285,7 +4285,7 @@
       <c r="I64" s="1"/>
       <c r="J64" s="4"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="2" t="s">
@@ -4304,7 +4304,7 @@
       <c r="I65" s="1"/>
       <c r="J65" s="4"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="2" t="s">
@@ -4323,7 +4323,7 @@
       <c r="I66" s="1"/>
       <c r="J66" s="4"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="2" t="s">
@@ -4342,7 +4342,7 @@
       <c r="I67" s="1"/>
       <c r="J67" s="4"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="2" t="s">
@@ -4361,7 +4361,7 @@
       <c r="I68" s="1"/>
       <c r="J68" s="4"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="2" t="s">
@@ -4380,7 +4380,7 @@
       <c r="I69" s="1"/>
       <c r="J69" s="4"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="2" t="s">
@@ -4399,7 +4399,7 @@
       <c r="I70" s="1"/>
       <c r="J70" s="4"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="2" t="s">
@@ -4418,7 +4418,7 @@
       <c r="I71" s="1"/>
       <c r="J71" s="4"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="2" t="s">
@@ -4437,7 +4437,7 @@
       <c r="I72" s="1"/>
       <c r="J72" s="4"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="2" t="s">
@@ -4456,7 +4456,7 @@
       <c r="I73" s="1"/>
       <c r="J73" s="4"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="2" t="s">
@@ -4475,7 +4475,7 @@
       <c r="I74" s="1"/>
       <c r="J74" s="4"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="2" t="s">
@@ -4494,7 +4494,7 @@
       <c r="I75" s="1"/>
       <c r="J75" s="4"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="2" t="s">
@@ -4513,7 +4513,7 @@
       <c r="I76" s="1"/>
       <c r="J76" s="4"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="2" t="s">
@@ -4532,7 +4532,7 @@
       <c r="I77" s="1"/>
       <c r="J77" s="4"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="2" t="s">
@@ -4551,7 +4551,7 @@
       <c r="I78" s="1"/>
       <c r="J78" s="4"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="2" t="s">
@@ -4570,7 +4570,7 @@
       <c r="I79" s="1"/>
       <c r="J79" s="4"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="2" t="s">
@@ -4589,7 +4589,7 @@
       <c r="I80" s="1"/>
       <c r="J80" s="4"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="2" t="s">
@@ -4608,7 +4608,7 @@
       <c r="I81" s="1"/>
       <c r="J81" s="4"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="2" t="s">
@@ -4627,7 +4627,7 @@
       <c r="I82" s="1"/>
       <c r="J82" s="4"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="2" t="s">
@@ -4648,7 +4648,7 @@
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="2" t="s">
@@ -4669,7 +4669,7 @@
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="2" t="s">
@@ -4690,7 +4690,7 @@
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="2" t="s">
@@ -4711,7 +4711,7 @@
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="2" t="s">
@@ -4732,7 +4732,7 @@
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="2" t="s">
@@ -4753,7 +4753,7 @@
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:10">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="2" t="s">
@@ -4774,7 +4774,7 @@
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="2" t="s">
@@ -4793,7 +4793,7 @@
       <c r="I90" s="1"/>
       <c r="J90" s="4"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="2" t="s">
@@ -4812,7 +4812,7 @@
       <c r="I91" s="1"/>
       <c r="J91" s="4"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="2" t="s">
@@ -4831,7 +4831,7 @@
       <c r="I92" s="1"/>
       <c r="J92" s="4"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="5" t="s">
@@ -4853,7 +4853,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="2" t="s">
@@ -4872,7 +4872,7 @@
       <c r="I94" s="1"/>
       <c r="J94" s="4"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:10">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="2" t="s">
@@ -4891,7 +4891,7 @@
       <c r="I95" s="1"/>
       <c r="J95" s="4"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:10">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="2" t="s">
@@ -4910,7 +4910,7 @@
       <c r="I96" s="1"/>
       <c r="J96" s="4"/>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:10">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="2" t="s">
@@ -4931,7 +4931,7 @@
       <c r="H97" s="1"/>
       <c r="I97" s="1"/>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="5" t="s">
@@ -4953,7 +4953,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:10">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="2" t="s">
@@ -4971,7 +4971,7 @@
       <c r="H99" s="1"/>
       <c r="I99" s="1"/>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:10">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="2" t="s">
@@ -4990,7 +4990,7 @@
       <c r="I100" s="1"/>
       <c r="J100" s="1"/>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:10">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="2" t="s">

</xml_diff>